<commit_message>
apply first successful tbox mode of data2rdf
</commit_message>
<xml_diff>
--- a/tests/tbox/xls_pipeline_test/input/data/classes.xlsx
+++ b/tests/tbox/xls_pipeline_test/input/data/classes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BUE\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BUE\data2rdf\tests\tbox\xls_pipeline_test\input\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>ModulusOfElasticity</t>
   </si>
@@ -61,15 +61,9 @@
     <t>Author's name</t>
   </si>
   <si>
-    <t>Author's email</t>
-  </si>
-  <si>
     <t>Original name</t>
   </si>
   <si>
-    <t>Ontological  concept ID</t>
-  </si>
-  <si>
     <t>Quotient of change of stress and change of extension in the range of evaluation in the elastic regime.</t>
   </si>
   <si>
@@ -80,9 +74,6 @@
   </si>
   <si>
     <t>Jane Doe</t>
-  </si>
-  <si>
-    <t>jane.doe@example.com</t>
   </si>
   <si>
     <t>Some comment</t>
@@ -126,17 +117,17 @@
     <t>John Doe</t>
   </si>
   <si>
-    <t>john.doe@example.com</t>
-  </si>
-  <si>
     <t xml:space="preserve">MPa </t>
+  </si>
+  <si>
+    <t>Ontological concept ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,14 +139,6 @@
       <b/>
       <sz val="11"/>
       <color theme="2"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -248,30 +231,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -604,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -619,21 +598,20 @@
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.1640625" customWidth="1"/>
     <col min="7" max="7" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.4140625" customWidth="1"/>
-    <col min="9" max="9" width="32.4140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.33203125" customWidth="1"/>
-    <col min="11" max="11" width="23.9140625" customWidth="1"/>
-    <col min="12" max="12" width="25.4140625" customWidth="1"/>
-    <col min="13" max="13" width="11" customWidth="1"/>
-    <col min="14" max="14" width="10.9140625" customWidth="1"/>
+    <col min="8" max="8" width="32.4140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" customWidth="1"/>
+    <col min="10" max="10" width="23.9140625" customWidth="1"/>
+    <col min="11" max="11" width="25.4140625" customWidth="1"/>
+    <col min="12" max="12" width="11" customWidth="1"/>
+    <col min="13" max="13" width="10.9140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -650,39 +628,33 @@
       <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="I1" s="4"/>
       <c r="J1" s="5"/>
-      <c r="K1" s="6"/>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>16</v>
+    <row r="2" spans="1:10">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -690,53 +662,43 @@
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="14.5">
+      <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="14.5">
-      <c r="A4" t="s">
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
         <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="H3" r:id="rId1"/>
-    <hyperlink ref="H4" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>